<commit_message>
Update the RPEpUACE in BLAPE file
</commit_message>
<xml_diff>
--- a/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
+++ b/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shigu\Documents\_swj\_Talanoa\CPSA Fletcher\dados\InputData (BR) 2024\d15 land\BLAPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssy02/Desktop/Postdoc Projects/eps-brazil-cpl/InputData/land/BLAPE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBB7102-3FDE-4D22-BBAA-A353EE588C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4222743-B16C-0D42-A968-34400E84F608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="2352" windowWidth="17220" windowHeight="9912" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -296,7 +296,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -308,20 +308,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -629,18 +629,18 @@
       <selection activeCell="A18" sqref="A18:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="51.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,42 +648,42 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -699,22 +699,22 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -736,25 +736,25 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -764,12 +764,12 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -779,22 +779,22 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
         <v>38</v>
       </c>
@@ -823,7 +823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
         <v>40</v>
       </c>
@@ -853,7 +853,7 @@
         <v>652321.40993903182</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
         <v>41</v>
       </c>
@@ -862,7 +862,7 @@
         <v>652321409939031.88</v>
       </c>
     </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J18" s="12"/>
     </row>
   </sheetData>
@@ -876,21 +876,21 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -898,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -922,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -946,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -962,23 +962,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="3">
-        <v>2.0200000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.3636084384378205E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3">
-        <v>8.0799999999999999E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1.335357177073511E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -999,16 +999,16 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="17" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>652321409939031.88</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2019,265 +2019,265 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="3">
         <f>B$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="C11" s="3">
         <f>C$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="D11" s="3">
         <f>D$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="E11" s="3">
         <f>E$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="F11" s="3">
         <f>F$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="G11" s="3">
         <f>G$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="H11" s="3">
         <f>H$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="I11" s="3">
         <f>I$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="J11" s="3">
         <f>J$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="K11" s="3">
         <f>K$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="L11" s="3">
         <f>L$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="M11" s="3">
         <f>M$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="N11" s="3">
         <f>N$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="O11" s="3">
         <f>O$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="P11" s="3">
         <f>P$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="Q11" s="3">
         <f>Q$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="R11" s="3">
         <f>R$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="S11" s="3">
         <f>S$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="T11" s="3">
         <f>T$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="U11" s="3">
         <f>U$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="V11" s="3">
         <f>V$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="W11" s="3">
         <f>W$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="X11" s="3">
         <f>X$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="Y11" s="3">
         <f>Y$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="Z11" s="3">
         <f>Z$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="AA11" s="3">
         <f>AA$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="AB11" s="3">
         <f>AB$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="AC11" s="3">
         <f>AC$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="AD11" s="3">
         <f>AD$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="AE11" s="3">
         <f>AE$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
+        <v>2846475208983.6162</v>
       </c>
       <c r="AF11" s="3">
         <f>AF$2*'data from RPEpUACE'!$B11</f>
-        <v>1317689248076.8445</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+        <v>2846475208983.6162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3">
         <f>B$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="C12" s="3">
         <f>C$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="D12" s="3">
         <f>D$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="E12" s="3">
         <f>E$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="F12" s="3">
         <f>F$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="G12" s="3">
         <f>G$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="H12" s="3">
         <f>H$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="I12" s="3">
         <f>I$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="J12" s="3">
         <f>J$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="K12" s="3">
         <f>K$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="L12" s="3">
         <f>L$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="M12" s="3">
         <f>M$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="N12" s="3">
         <f>N$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="O12" s="3">
         <f>O$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="P12" s="3">
         <f>P$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="Q12" s="3">
         <f>Q$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="R12" s="3">
         <f>R$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="S12" s="3">
         <f>S$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="T12" s="3">
         <f>T$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="U12" s="3">
         <f>U$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="V12" s="3">
         <f>V$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="W12" s="3">
         <f>W$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="X12" s="3">
         <f>X$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="Y12" s="3">
         <f>Y$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="Z12" s="3">
         <f>Z$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="AA12" s="3">
         <f>AA$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="AB12" s="3">
         <f>AB$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="AC12" s="3">
         <f>AC$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="AD12" s="3">
         <f>AD$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="AE12" s="3">
         <f>AE$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
+        <v>87108207652.079819</v>
       </c>
       <c r="AF12" s="3">
         <f>AF$2*'data from RPEpUACE'!$B12</f>
-        <v>52707569923.073776</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+        <v>87108207652.079819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>

</xml_diff>